<commit_message>
fix kopeyki and punkt
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -48,18 +48,6 @@
     <t>остаток</t>
   </si>
   <si>
-    <t>договор 177-ALNG2-2020/05-ОРСО от 21.02.2023</t>
-  </si>
-  <si>
-    <t>Договор № 0091.2019АГХК/2/Велесстрой/02-Пр-ОРСО от 01.09.2021 года</t>
-  </si>
-  <si>
-    <t>договор 619-ЮР-2019/10-ОРСО</t>
-  </si>
-  <si>
-    <t>Договор № 0091.2019АГХК/2/Велесстрой/02-Ст-ОРСО от 01.09.2021 года</t>
-  </si>
-  <si>
     <t>Итого по договорам:</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t>Остаток по договору:</t>
   </si>
   <si>
-    <t>Велестрой</t>
-  </si>
-  <si>
     <t>Мы должны</t>
   </si>
   <si>
@@ -79,6 +64,21 @@
   </si>
   <si>
     <t>да</t>
+  </si>
+  <si>
+    <t>ООО "Крафт-Электро"</t>
+  </si>
+  <si>
+    <t>Договор № 150/З-ЭС/2023д от 01.07.2023 г.</t>
+  </si>
+  <si>
+    <t>Договор № 95.1-ЭС/2023д от 23.05.2023 г.</t>
+  </si>
+  <si>
+    <t>Договор № 95.2-ЭС/2023д от 23.05.2023 г.</t>
+  </si>
+  <si>
+    <t>Договор № 95-ЭС2023о от 23.06.2023 г</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="11">
-        <v>45203</v>
+        <v>45233</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1080,22 +1080,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B12" s="71"/>
       <c r="C12" s="72" t="str">
         <f>CONCATENATE("Задолженность ЗАО ""ЭнергоСтрой"" перед ",B7)</f>
-        <v>Задолженность ЗАО "ЭнергоСтрой" перед Велестрой</v>
+        <v>Задолженность ЗАО "ЭнергоСтрой" перед ООО "Крафт-Электро"</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="70" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G12" s="71"/>
       <c r="H12" s="74" t="str">
         <f>CONCATENATE(B7,"  перед ЗАО ""Энергострой""")</f>
-        <v>Велестрой  перед ЗАО "Энергострой"</v>
+        <v>ООО "Крафт-Электро"  перед ЗАО "Энергострой"</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -1128,72 +1128,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" s="18">
-        <v>14028068.32</v>
+        <v>183048.19</v>
       </c>
       <c r="D14" s="18">
-        <v>2</v>
+        <v>183048.19</v>
       </c>
       <c r="E14" s="68">
         <f>C14-D14</f>
-        <v>14028066.32</v>
+        <v>0</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H14" s="18">
-        <v>1567980.25</v>
+        <v>4040</v>
       </c>
       <c r="I14" s="18">
-        <v>1567980.25</v>
+        <v>4040</v>
       </c>
       <c r="J14" s="68">
         <f>H14-I14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="18">
-        <v>82123435.200000003</v>
-      </c>
-      <c r="D15" s="18">
-        <v>82123435.200000003</v>
-      </c>
-      <c r="E15" s="68">
-        <f t="shared" ref="E15" si="0">C15-D15</f>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="18">
+        <v>66549.16</v>
+      </c>
+      <c r="I15" s="18">
+        <v>66549.16</v>
+      </c>
+      <c r="J15" s="68">
+        <f t="shared" ref="J15:J16" si="0">H15-I15</f>
         <v>0</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="18">
-        <v>3406704.84</v>
-      </c>
-      <c r="I15" s="18">
-        <v>1567980.25</v>
-      </c>
-      <c r="J15" s="68">
-        <f t="shared" ref="J15" si="1">H15-I15</f>
-        <v>1838724.5899999999</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1202,11 +1191,22 @@
       <c r="C16" s="18"/>
       <c r="D16" s="23"/>
       <c r="E16" s="68"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="68"/>
+      <c r="F16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="18">
+        <v>248922.74</v>
+      </c>
+      <c r="I16" s="18">
+        <v>112459.03</v>
+      </c>
+      <c r="J16" s="68">
+        <f t="shared" si="0"/>
+        <v>136463.71</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17"/>
@@ -1618,36 +1618,36 @@
     </row>
     <row r="51" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B51" s="30"/>
       <c r="C51" s="31">
         <f>SUM(C14:C50)</f>
-        <v>96151503.520000011</v>
+        <v>183048.19</v>
       </c>
       <c r="D51" s="31">
         <f>SUM(D14:D50)</f>
-        <v>82123437.200000003</v>
+        <v>183048.19</v>
       </c>
       <c r="E51" s="31">
-        <f t="shared" ref="E51" si="2">SUM(E14:E50)</f>
-        <v>14028066.32</v>
+        <f>SUM(E14:E50)</f>
+        <v>0</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G51" s="29"/>
       <c r="H51" s="32">
         <f>SUM(H14:H50)</f>
-        <v>4974685.09</v>
+        <v>319511.90000000002</v>
       </c>
       <c r="I51" s="31">
         <f>SUM(I14:I50)</f>
-        <v>3135960.5</v>
+        <v>183048.19</v>
       </c>
       <c r="J51" s="31">
         <f>SUM(J14:J50)</f>
-        <v>1838724.5899999999</v>
+        <v>136463.71</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -1664,20 +1664,20 @@
     </row>
     <row r="53" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="39" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B53" s="40"/>
       <c r="C53" s="41">
-        <f>H51</f>
-        <v>4974685.09</v>
+        <f>J51</f>
+        <v>136463.71</v>
       </c>
       <c r="D53" s="42"/>
       <c r="E53" s="42"/>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
       <c r="H53" s="41">
-        <f>C53</f>
-        <v>4974685.09</v>
+        <f>J51</f>
+        <v>136463.71</v>
       </c>
       <c r="I53" s="42"/>
       <c r="J53" s="42"/>
@@ -1696,22 +1696,22 @@
     </row>
     <row r="55" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B55" s="51"/>
       <c r="C55" s="52">
         <f>C51-C53</f>
-        <v>91176818.430000007</v>
+        <v>46584.48000000001</v>
       </c>
       <c r="D55" s="53"/>
       <c r="E55" s="53"/>
       <c r="F55" s="54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G55" s="54"/>
       <c r="H55" s="55">
         <f>H51-H53</f>
-        <v>0</v>
+        <v>183048.19000000003</v>
       </c>
       <c r="I55" s="53"/>
       <c r="J55" s="53"/>

</xml_diff>